<commit_message>
Change Schedule for Jennifer
Jennifer의 의견으로 일정 추가 및 변경
</commit_message>
<xml_diff>
--- a/Product Launching Documentation_0303_rev1.xlsx
+++ b/Product Launching Documentation_0303_rev1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="226">
   <si>
     <t>SW downloads, release and general information</t>
   </si>
@@ -889,61 +889,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>영문</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>문서</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>작성</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C9516 Training support</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Comcast Presentation</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -969,10 +914,6 @@
   </si>
   <si>
     <t>최초 작성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>감수</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1163,8 +1104,93 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>C9500 Installation Guides</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C9504N Installation Guides</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C1004P Quick Installation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C1004P Data Sheet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>감수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>최초 작성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C9516 Training Kit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Feedback </t>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>월</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>일</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>전달</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -1236,15 +1262,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>C9500 Installation Guides</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C9504N Installation Guides</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>한글 문서 취합</t>
+    <t>C1004 Quick Installation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C1004W Quick Installation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C1004WA Data Sheet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한글 문서 취합 / 영문문서 작성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C9504N User Manual</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1407,7 +1441,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="89">
+  <borders count="75">
     <border>
       <left/>
       <right/>
@@ -2231,19 +2265,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color theme="1"/>
@@ -2320,51 +2341,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color theme="1"/>
       </left>
@@ -2381,88 +2357,6 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
@@ -2493,69 +2387,6 @@
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2575,14 +2406,25 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
-        <color theme="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="medium">
         <color indexed="64"/>
@@ -2593,7 +2435,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="193">
+  <cellXfs count="181">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2810,29 +2652,11 @@
     <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -2852,13 +2676,13 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2885,115 +2709,55 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="86" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="87" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="88" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="8" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="79" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="6" borderId="79" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="8" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3005,6 +2769,15 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3014,15 +2787,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3032,23 +2796,83 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3056,88 +2880,40 @@
     <xf numFmtId="177" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="85" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="6" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="8" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="8" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3158,13 +2934,43 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3300,13 +3106,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>76201</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>69</xdr:row>
       <xdr:rowOff>57151</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1666876</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>72</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3373,13 +3179,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>178971</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>169446</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>72</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3435,13 +3241,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>178971</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>69</xdr:row>
       <xdr:rowOff>131846</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>169875</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>94065</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3751,7 +3557,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3762,14 +3568,14 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O61"/>
+  <dimension ref="A1:O69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.625" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.25" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" style="10" bestFit="1" customWidth="1"/>
     <col min="3" max="7" width="6.25" style="10" customWidth="1"/>
     <col min="8" max="15" width="6.875" style="7" customWidth="1"/>
     <col min="16" max="16384" width="9" style="8"/>
@@ -3785,46 +3591,46 @@
       <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="142" t="s">
+      <c r="A2" s="104" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="148" t="s">
+      <c r="B2" s="107" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="136" t="s">
+      <c r="C2" s="110" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="151" t="s">
+      <c r="D2" s="113" t="s">
         <v>166</v>
       </c>
-      <c r="E2" s="151" t="s">
+      <c r="E2" s="113" t="s">
         <v>167</v>
       </c>
-      <c r="F2" s="139" t="s">
+      <c r="F2" s="116" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="139" t="s">
+      <c r="G2" s="116" t="s">
         <v>169</v>
       </c>
-      <c r="H2" s="145" t="s">
+      <c r="H2" s="119" t="s">
         <v>56</v>
       </c>
-      <c r="I2" s="146"/>
-      <c r="J2" s="146"/>
-      <c r="K2" s="146"/>
-      <c r="L2" s="146"/>
-      <c r="M2" s="146"/>
-      <c r="N2" s="146"/>
-      <c r="O2" s="147"/>
+      <c r="I2" s="120"/>
+      <c r="J2" s="120"/>
+      <c r="K2" s="120"/>
+      <c r="L2" s="120"/>
+      <c r="M2" s="120"/>
+      <c r="N2" s="120"/>
+      <c r="O2" s="121"/>
     </row>
     <row r="3" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="143"/>
-      <c r="B3" s="149"/>
-      <c r="C3" s="137"/>
-      <c r="D3" s="152"/>
-      <c r="E3" s="152"/>
-      <c r="F3" s="140"/>
-      <c r="G3" s="140"/>
+      <c r="A3" s="105"/>
+      <c r="B3" s="108"/>
+      <c r="C3" s="111"/>
+      <c r="D3" s="114"/>
+      <c r="E3" s="114"/>
+      <c r="F3" s="117"/>
+      <c r="G3" s="117"/>
       <c r="H3" s="60">
         <v>1</v>
       </c>
@@ -3851,13 +3657,13 @@
       </c>
     </row>
     <row r="4" spans="1:15" s="9" customFormat="1" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="144"/>
-      <c r="B4" s="150"/>
-      <c r="C4" s="138"/>
-      <c r="D4" s="153"/>
-      <c r="E4" s="153"/>
-      <c r="F4" s="141"/>
-      <c r="G4" s="141"/>
+      <c r="A4" s="106"/>
+      <c r="B4" s="109"/>
+      <c r="C4" s="112"/>
+      <c r="D4" s="115"/>
+      <c r="E4" s="115"/>
+      <c r="F4" s="118"/>
+      <c r="G4" s="118"/>
       <c r="H4" s="49" t="s">
         <v>45</v>
       </c>
@@ -4130,27 +3936,27 @@
     </row>
     <row r="16" spans="1:15" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:15" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="88"/>
-      <c r="B17" s="89" t="s">
-        <v>205</v>
-      </c>
-      <c r="C17" s="173">
+      <c r="A17" s="82"/>
+      <c r="B17" s="83" t="s">
+        <v>203</v>
+      </c>
+      <c r="C17" s="98">
         <v>6</v>
       </c>
-      <c r="D17" s="174"/>
-      <c r="E17" s="89"/>
-      <c r="F17" s="89"/>
-      <c r="G17" s="89"/>
-      <c r="H17" s="90"/>
-      <c r="I17" s="176" t="s">
-        <v>212</v>
-      </c>
-      <c r="J17" s="177"/>
-      <c r="K17" s="177"/>
-      <c r="L17" s="177"/>
-      <c r="M17" s="177"/>
-      <c r="N17" s="177"/>
-      <c r="O17" s="178"/>
+      <c r="D17" s="99"/>
+      <c r="E17" s="83"/>
+      <c r="F17" s="83"/>
+      <c r="G17" s="83"/>
+      <c r="H17" s="84"/>
+      <c r="I17" s="101" t="s">
+        <v>209</v>
+      </c>
+      <c r="J17" s="102"/>
+      <c r="K17" s="102"/>
+      <c r="L17" s="102"/>
+      <c r="M17" s="102"/>
+      <c r="N17" s="102"/>
+      <c r="O17" s="103"/>
     </row>
     <row r="18" spans="1:15" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4160,27 +3966,27 @@
       <c r="B19" s="65" t="s">
         <v>187</v>
       </c>
-      <c r="C19" s="159" t="s">
-        <v>204</v>
-      </c>
-      <c r="D19" s="128"/>
-      <c r="E19" s="128" t="s">
+      <c r="C19" s="129" t="s">
+        <v>202</v>
+      </c>
+      <c r="D19" s="130"/>
+      <c r="E19" s="130" t="s">
         <v>177</v>
       </c>
-      <c r="F19" s="128"/>
-      <c r="G19" s="128" t="s">
+      <c r="F19" s="130"/>
+      <c r="G19" s="130" t="s">
         <v>178</v>
       </c>
-      <c r="H19" s="128"/>
-      <c r="I19" s="129" t="s">
+      <c r="H19" s="130"/>
+      <c r="I19" s="144" t="s">
         <v>191</v>
       </c>
-      <c r="J19" s="128"/>
-      <c r="K19" s="128"/>
-      <c r="L19" s="128"/>
-      <c r="M19" s="128"/>
-      <c r="N19" s="128"/>
-      <c r="O19" s="130"/>
+      <c r="J19" s="130"/>
+      <c r="K19" s="130"/>
+      <c r="L19" s="130"/>
+      <c r="M19" s="130"/>
+      <c r="N19" s="130"/>
+      <c r="O19" s="145"/>
     </row>
     <row r="20" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="51">
@@ -4189,27 +3995,27 @@
       <c r="B20" s="66" t="s">
         <v>176</v>
       </c>
-      <c r="C20" s="131">
+      <c r="C20" s="137">
         <v>2</v>
       </c>
-      <c r="D20" s="132"/>
-      <c r="E20" s="133">
+      <c r="D20" s="138"/>
+      <c r="E20" s="146">
         <v>42431</v>
       </c>
-      <c r="F20" s="133"/>
-      <c r="G20" s="133">
+      <c r="F20" s="146"/>
+      <c r="G20" s="146">
         <v>42431</v>
       </c>
-      <c r="H20" s="134"/>
-      <c r="I20" s="134" t="s">
+      <c r="H20" s="147"/>
+      <c r="I20" s="147" t="s">
         <v>192</v>
       </c>
-      <c r="J20" s="134"/>
-      <c r="K20" s="134"/>
-      <c r="L20" s="134"/>
-      <c r="M20" s="134"/>
-      <c r="N20" s="134"/>
-      <c r="O20" s="135"/>
+      <c r="J20" s="147"/>
+      <c r="K20" s="147"/>
+      <c r="L20" s="147"/>
+      <c r="M20" s="147"/>
+      <c r="N20" s="147"/>
+      <c r="O20" s="151"/>
     </row>
     <row r="21" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="52">
@@ -4218,27 +4024,27 @@
       <c r="B21" s="67" t="s">
         <v>179</v>
       </c>
-      <c r="C21" s="105">
+      <c r="C21" s="139">
         <v>2</v>
       </c>
-      <c r="D21" s="109"/>
-      <c r="E21" s="110">
+      <c r="D21" s="140"/>
+      <c r="E21" s="127">
         <v>42431</v>
       </c>
-      <c r="F21" s="110"/>
-      <c r="G21" s="110">
+      <c r="F21" s="127"/>
+      <c r="G21" s="127">
         <v>42431</v>
       </c>
-      <c r="H21" s="111"/>
-      <c r="I21" s="111" t="s">
+      <c r="H21" s="128"/>
+      <c r="I21" s="128" t="s">
         <v>192</v>
       </c>
-      <c r="J21" s="111"/>
-      <c r="K21" s="111"/>
-      <c r="L21" s="111"/>
-      <c r="M21" s="111"/>
-      <c r="N21" s="111"/>
-      <c r="O21" s="115"/>
+      <c r="J21" s="128"/>
+      <c r="K21" s="128"/>
+      <c r="L21" s="128"/>
+      <c r="M21" s="128"/>
+      <c r="N21" s="128"/>
+      <c r="O21" s="150"/>
     </row>
     <row r="22" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="52">
@@ -4247,140 +4053,140 @@
       <c r="B22" s="67" t="s">
         <v>180</v>
       </c>
-      <c r="C22" s="121">
+      <c r="C22" s="135">
         <v>3</v>
       </c>
-      <c r="D22" s="109"/>
-      <c r="E22" s="110">
+      <c r="D22" s="140"/>
+      <c r="E22" s="127">
         <v>42432</v>
       </c>
-      <c r="F22" s="110"/>
-      <c r="G22" s="110">
+      <c r="F22" s="127"/>
+      <c r="G22" s="127">
         <v>42432</v>
       </c>
-      <c r="H22" s="111"/>
-      <c r="I22" s="111" t="s">
+      <c r="H22" s="128"/>
+      <c r="I22" s="128" t="s">
         <v>193</v>
       </c>
-      <c r="J22" s="111"/>
-      <c r="K22" s="111"/>
-      <c r="L22" s="111"/>
-      <c r="M22" s="111"/>
-      <c r="N22" s="111"/>
-      <c r="O22" s="115"/>
+      <c r="J22" s="128"/>
+      <c r="K22" s="128"/>
+      <c r="L22" s="128"/>
+      <c r="M22" s="128"/>
+      <c r="N22" s="128"/>
+      <c r="O22" s="150"/>
     </row>
     <row r="23" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="52">
         <v>4</v>
       </c>
-      <c r="B23" s="98" t="s">
-        <v>202</v>
-      </c>
-      <c r="C23" s="116">
+      <c r="B23" s="92" t="s">
+        <v>219</v>
+      </c>
+      <c r="C23" s="153">
         <v>10</v>
       </c>
-      <c r="D23" s="116"/>
-      <c r="E23" s="117">
+      <c r="D23" s="153"/>
+      <c r="E23" s="154">
         <v>42432</v>
       </c>
-      <c r="F23" s="118"/>
-      <c r="G23" s="119">
+      <c r="F23" s="155"/>
+      <c r="G23" s="156">
         <v>42436</v>
       </c>
-      <c r="H23" s="119"/>
-      <c r="I23" s="120" t="s">
-        <v>216</v>
-      </c>
-      <c r="J23" s="121"/>
-      <c r="K23" s="121"/>
-      <c r="L23" s="121"/>
-      <c r="M23" s="121"/>
-      <c r="N23" s="121"/>
-      <c r="O23" s="122"/>
+      <c r="H23" s="156"/>
+      <c r="I23" s="134" t="s">
+        <v>220</v>
+      </c>
+      <c r="J23" s="135"/>
+      <c r="K23" s="135"/>
+      <c r="L23" s="135"/>
+      <c r="M23" s="135"/>
+      <c r="N23" s="135"/>
+      <c r="O23" s="136"/>
     </row>
     <row r="24" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="53">
         <v>5</v>
       </c>
       <c r="B24" s="67" t="s">
-        <v>213</v>
-      </c>
-      <c r="C24" s="105">
+        <v>210</v>
+      </c>
+      <c r="C24" s="139">
         <v>20</v>
       </c>
-      <c r="D24" s="106"/>
-      <c r="E24" s="110">
+      <c r="D24" s="141"/>
+      <c r="E24" s="127">
         <v>42433</v>
       </c>
-      <c r="F24" s="110"/>
-      <c r="G24" s="110">
+      <c r="F24" s="127"/>
+      <c r="G24" s="127">
         <v>42436</v>
       </c>
-      <c r="H24" s="111"/>
-      <c r="I24" s="111" t="s">
-        <v>215</v>
-      </c>
-      <c r="J24" s="111"/>
-      <c r="K24" s="111"/>
-      <c r="L24" s="111"/>
-      <c r="M24" s="111"/>
-      <c r="N24" s="111"/>
-      <c r="O24" s="115"/>
+      <c r="H24" s="128"/>
+      <c r="I24" s="128" t="s">
+        <v>212</v>
+      </c>
+      <c r="J24" s="128"/>
+      <c r="K24" s="128"/>
+      <c r="L24" s="128"/>
+      <c r="M24" s="128"/>
+      <c r="N24" s="128"/>
+      <c r="O24" s="150"/>
     </row>
     <row r="25" spans="1:15" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="54">
         <v>6</v>
       </c>
       <c r="B25" s="68" t="s">
-        <v>214</v>
-      </c>
-      <c r="C25" s="160">
+        <v>211</v>
+      </c>
+      <c r="C25" s="142">
         <v>10</v>
       </c>
-      <c r="D25" s="161"/>
-      <c r="E25" s="158">
+      <c r="D25" s="143"/>
+      <c r="E25" s="133">
         <v>42436</v>
       </c>
-      <c r="F25" s="158"/>
-      <c r="G25" s="158">
+      <c r="F25" s="133"/>
+      <c r="G25" s="133">
         <v>42437</v>
       </c>
-      <c r="H25" s="156"/>
-      <c r="I25" s="156" t="s">
-        <v>215</v>
-      </c>
-      <c r="J25" s="156"/>
-      <c r="K25" s="156"/>
-      <c r="L25" s="156"/>
-      <c r="M25" s="156"/>
-      <c r="N25" s="156"/>
-      <c r="O25" s="157"/>
+      <c r="H25" s="131"/>
+      <c r="I25" s="131" t="s">
+        <v>212</v>
+      </c>
+      <c r="J25" s="131"/>
+      <c r="K25" s="131"/>
+      <c r="L25" s="131"/>
+      <c r="M25" s="131"/>
+      <c r="N25" s="131"/>
+      <c r="O25" s="132"/>
     </row>
     <row r="26" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="78"/>
+      <c r="A26" s="69"/>
       <c r="B26" s="71"/>
-      <c r="C26" s="154">
+      <c r="C26" s="148">
         <f>SUM(C20:D25)</f>
         <v>47</v>
       </c>
-      <c r="D26" s="154"/>
-      <c r="E26" s="155">
+      <c r="D26" s="148"/>
+      <c r="E26" s="149">
         <f>ROUNDUP(C26/(8 + 4), 0)</f>
         <v>4</v>
       </c>
-      <c r="F26" s="155"/>
-      <c r="G26" s="76"/>
-      <c r="H26" s="77"/>
-      <c r="I26" s="77"/>
-      <c r="J26" s="77"/>
-      <c r="K26" s="77"/>
-      <c r="L26" s="77"/>
-      <c r="M26" s="77"/>
-      <c r="N26" s="77"/>
-      <c r="O26" s="77"/>
+      <c r="F26" s="149"/>
+      <c r="G26" s="74"/>
+      <c r="H26" s="75"/>
+      <c r="I26" s="75"/>
+      <c r="J26" s="75"/>
+      <c r="K26" s="75"/>
+      <c r="L26" s="75"/>
+      <c r="M26" s="75"/>
+      <c r="N26" s="75"/>
+      <c r="O26" s="75"/>
     </row>
     <row r="27" spans="1:15" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="75"/>
+      <c r="A27" s="69"/>
       <c r="B27" s="71"/>
       <c r="C27" s="72"/>
       <c r="D27" s="72"/>
@@ -4403,143 +4209,143 @@
       <c r="B28" s="65" t="s">
         <v>187</v>
       </c>
-      <c r="C28" s="159" t="s">
-        <v>204</v>
-      </c>
-      <c r="D28" s="128"/>
-      <c r="E28" s="128" t="s">
+      <c r="C28" s="129" t="s">
+        <v>202</v>
+      </c>
+      <c r="D28" s="130"/>
+      <c r="E28" s="130" t="s">
         <v>177</v>
       </c>
-      <c r="F28" s="128"/>
-      <c r="G28" s="128" t="s">
+      <c r="F28" s="130"/>
+      <c r="G28" s="130" t="s">
         <v>178</v>
       </c>
-      <c r="H28" s="128"/>
-      <c r="I28" s="129" t="s">
+      <c r="H28" s="130"/>
+      <c r="I28" s="144" t="s">
         <v>191</v>
       </c>
-      <c r="J28" s="128"/>
-      <c r="K28" s="128"/>
-      <c r="L28" s="128"/>
-      <c r="M28" s="128"/>
-      <c r="N28" s="128"/>
-      <c r="O28" s="130"/>
+      <c r="J28" s="130"/>
+      <c r="K28" s="130"/>
+      <c r="L28" s="130"/>
+      <c r="M28" s="130"/>
+      <c r="N28" s="130"/>
+      <c r="O28" s="145"/>
     </row>
     <row r="29" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="51">
         <v>7</v>
       </c>
       <c r="B29" s="66" t="s">
-        <v>217</v>
-      </c>
-      <c r="C29" s="131">
+        <v>213</v>
+      </c>
+      <c r="C29" s="137">
         <v>2</v>
       </c>
-      <c r="D29" s="132"/>
-      <c r="E29" s="133">
+      <c r="D29" s="138"/>
+      <c r="E29" s="146">
         <v>42438</v>
       </c>
-      <c r="F29" s="133"/>
-      <c r="G29" s="133">
+      <c r="F29" s="146"/>
+      <c r="G29" s="146">
         <v>42438</v>
       </c>
-      <c r="H29" s="134"/>
-      <c r="I29" s="134" t="s">
+      <c r="H29" s="147"/>
+      <c r="I29" s="147" t="s">
         <v>192</v>
       </c>
-      <c r="J29" s="134"/>
-      <c r="K29" s="134"/>
-      <c r="L29" s="134"/>
-      <c r="M29" s="134"/>
-      <c r="N29" s="134"/>
-      <c r="O29" s="135"/>
+      <c r="J29" s="147"/>
+      <c r="K29" s="147"/>
+      <c r="L29" s="147"/>
+      <c r="M29" s="147"/>
+      <c r="N29" s="147"/>
+      <c r="O29" s="151"/>
     </row>
     <row r="30" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="52">
         <v>8</v>
       </c>
-      <c r="B30" s="67" t="s">
-        <v>181</v>
-      </c>
-      <c r="C30" s="105">
+      <c r="B30" s="93" t="s">
+        <v>215</v>
+      </c>
+      <c r="C30" s="139">
         <v>2</v>
       </c>
-      <c r="D30" s="106"/>
-      <c r="E30" s="107">
+      <c r="D30" s="141"/>
+      <c r="E30" s="125">
         <v>42438</v>
       </c>
-      <c r="F30" s="108"/>
-      <c r="G30" s="107">
+      <c r="F30" s="126"/>
+      <c r="G30" s="125">
         <v>42438</v>
       </c>
-      <c r="H30" s="108"/>
-      <c r="I30" s="120" t="s">
-        <v>192</v>
-      </c>
-      <c r="J30" s="121"/>
-      <c r="K30" s="121"/>
-      <c r="L30" s="121"/>
-      <c r="M30" s="121"/>
-      <c r="N30" s="121"/>
-      <c r="O30" s="122"/>
+      <c r="H30" s="126"/>
+      <c r="I30" s="168" t="s">
+        <v>217</v>
+      </c>
+      <c r="J30" s="135"/>
+      <c r="K30" s="135"/>
+      <c r="L30" s="135"/>
+      <c r="M30" s="135"/>
+      <c r="N30" s="135"/>
+      <c r="O30" s="136"/>
     </row>
     <row r="31" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="53">
         <v>9</v>
       </c>
-      <c r="B31" s="67" t="s">
-        <v>183</v>
-      </c>
-      <c r="C31" s="105">
+      <c r="B31" s="93" t="s">
+        <v>206</v>
+      </c>
+      <c r="C31" s="139">
         <v>2</v>
       </c>
-      <c r="D31" s="106"/>
-      <c r="E31" s="107">
+      <c r="D31" s="141"/>
+      <c r="E31" s="125">
         <v>42438</v>
       </c>
-      <c r="F31" s="108"/>
-      <c r="G31" s="107">
+      <c r="F31" s="126"/>
+      <c r="G31" s="125">
         <v>42438</v>
       </c>
-      <c r="H31" s="108"/>
-      <c r="I31" s="120" t="s">
+      <c r="H31" s="126"/>
+      <c r="I31" s="134" t="s">
         <v>192</v>
       </c>
-      <c r="J31" s="121"/>
-      <c r="K31" s="121"/>
-      <c r="L31" s="121"/>
-      <c r="M31" s="121"/>
-      <c r="N31" s="121"/>
-      <c r="O31" s="122"/>
+      <c r="J31" s="135"/>
+      <c r="K31" s="135"/>
+      <c r="L31" s="135"/>
+      <c r="M31" s="135"/>
+      <c r="N31" s="135"/>
+      <c r="O31" s="136"/>
     </row>
     <row r="32" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="53">
         <v>10</v>
       </c>
-      <c r="B32" s="101" t="s">
-        <v>208</v>
-      </c>
-      <c r="C32" s="112">
-        <v>2</v>
-      </c>
-      <c r="D32" s="113"/>
-      <c r="E32" s="107">
+      <c r="B32" s="93" t="s">
+        <v>216</v>
+      </c>
+      <c r="C32" s="122">
+        <v>6</v>
+      </c>
+      <c r="D32" s="123"/>
+      <c r="E32" s="125">
         <v>42438</v>
       </c>
-      <c r="F32" s="108"/>
-      <c r="G32" s="107">
+      <c r="F32" s="126"/>
+      <c r="G32" s="125">
         <v>42438</v>
       </c>
-      <c r="H32" s="108"/>
-      <c r="I32" s="126" t="s">
-        <v>210</v>
-      </c>
-      <c r="J32" s="113"/>
-      <c r="K32" s="113"/>
-      <c r="L32" s="113"/>
-      <c r="M32" s="113"/>
-      <c r="N32" s="113"/>
-      <c r="O32" s="127"/>
+      <c r="H32" s="126"/>
+      <c r="I32" s="159" t="s">
+        <v>218</v>
+      </c>
+      <c r="J32" s="123"/>
+      <c r="K32" s="123"/>
+      <c r="L32" s="123"/>
+      <c r="M32" s="123"/>
+      <c r="N32" s="123"/>
+      <c r="O32" s="124"/>
     </row>
     <row r="33" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="52">
@@ -4548,27 +4354,27 @@
       <c r="B33" s="67" t="s">
         <v>182</v>
       </c>
-      <c r="C33" s="105">
+      <c r="C33" s="139">
         <v>2</v>
       </c>
-      <c r="D33" s="106"/>
-      <c r="E33" s="107">
+      <c r="D33" s="141"/>
+      <c r="E33" s="125">
         <v>42438</v>
       </c>
-      <c r="F33" s="108"/>
-      <c r="G33" s="107">
+      <c r="F33" s="126"/>
+      <c r="G33" s="125">
         <v>42438</v>
       </c>
-      <c r="H33" s="108"/>
-      <c r="I33" s="120" t="s">
+      <c r="H33" s="126"/>
+      <c r="I33" s="134" t="s">
         <v>192</v>
       </c>
-      <c r="J33" s="121"/>
-      <c r="K33" s="121"/>
-      <c r="L33" s="121"/>
-      <c r="M33" s="121"/>
-      <c r="N33" s="121"/>
-      <c r="O33" s="122"/>
+      <c r="J33" s="135"/>
+      <c r="K33" s="135"/>
+      <c r="L33" s="135"/>
+      <c r="M33" s="135"/>
+      <c r="N33" s="135"/>
+      <c r="O33" s="136"/>
     </row>
     <row r="34" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="52">
@@ -4577,228 +4383,232 @@
       <c r="B34" s="67" t="s">
         <v>184</v>
       </c>
-      <c r="C34" s="105">
+      <c r="C34" s="139">
         <v>2</v>
       </c>
-      <c r="D34" s="106"/>
-      <c r="E34" s="107">
-        <v>42438</v>
-      </c>
-      <c r="F34" s="108"/>
-      <c r="G34" s="107">
-        <v>42438</v>
-      </c>
-      <c r="H34" s="108"/>
-      <c r="I34" s="120" t="s">
+      <c r="D34" s="141"/>
+      <c r="E34" s="125">
+        <v>42439</v>
+      </c>
+      <c r="F34" s="126"/>
+      <c r="G34" s="125">
+        <v>42439</v>
+      </c>
+      <c r="H34" s="126"/>
+      <c r="I34" s="134" t="s">
         <v>192</v>
       </c>
-      <c r="J34" s="121"/>
-      <c r="K34" s="121"/>
-      <c r="L34" s="121"/>
-      <c r="M34" s="121"/>
-      <c r="N34" s="121"/>
-      <c r="O34" s="122"/>
+      <c r="J34" s="135"/>
+      <c r="K34" s="135"/>
+      <c r="L34" s="135"/>
+      <c r="M34" s="135"/>
+      <c r="N34" s="135"/>
+      <c r="O34" s="136"/>
     </row>
     <row r="35" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="52">
         <v>13</v>
       </c>
       <c r="B35" s="67" t="s">
-        <v>185</v>
-      </c>
-      <c r="C35" s="105">
-        <v>2</v>
-      </c>
-      <c r="D35" s="109"/>
-      <c r="E35" s="110">
+        <v>221</v>
+      </c>
+      <c r="C35" s="139">
+        <v>5</v>
+      </c>
+      <c r="D35" s="140"/>
+      <c r="E35" s="127">
         <v>42439</v>
       </c>
-      <c r="F35" s="110"/>
-      <c r="G35" s="110">
+      <c r="F35" s="127"/>
+      <c r="G35" s="127">
         <v>42439</v>
       </c>
-      <c r="H35" s="111"/>
-      <c r="I35" s="111" t="s">
-        <v>194</v>
-      </c>
-      <c r="J35" s="111"/>
-      <c r="K35" s="111"/>
-      <c r="L35" s="111"/>
-      <c r="M35" s="111"/>
-      <c r="N35" s="111"/>
-      <c r="O35" s="115"/>
+      <c r="H35" s="128"/>
+      <c r="I35" s="152" t="s">
+        <v>218</v>
+      </c>
+      <c r="J35" s="128"/>
+      <c r="K35" s="128"/>
+      <c r="L35" s="128"/>
+      <c r="M35" s="128"/>
+      <c r="N35" s="128"/>
+      <c r="O35" s="150"/>
     </row>
     <row r="36" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="52">
         <v>14</v>
       </c>
       <c r="B36" s="67" t="s">
+        <v>185</v>
+      </c>
+      <c r="C36" s="139">
+        <v>2</v>
+      </c>
+      <c r="D36" s="140"/>
+      <c r="E36" s="127">
+        <v>42439</v>
+      </c>
+      <c r="F36" s="127"/>
+      <c r="G36" s="127">
+        <v>42439</v>
+      </c>
+      <c r="H36" s="128"/>
+      <c r="I36" s="128" t="s">
+        <v>194</v>
+      </c>
+      <c r="J36" s="128"/>
+      <c r="K36" s="128"/>
+      <c r="L36" s="128"/>
+      <c r="M36" s="128"/>
+      <c r="N36" s="128"/>
+      <c r="O36" s="150"/>
+    </row>
+    <row r="37" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="52">
+        <v>15</v>
+      </c>
+      <c r="B37" s="67" t="s">
         <v>186</v>
       </c>
-      <c r="C36" s="105">
+      <c r="C37" s="139">
         <v>2</v>
       </c>
-      <c r="D36" s="109"/>
-      <c r="E36" s="110">
+      <c r="D37" s="140"/>
+      <c r="E37" s="127">
         <v>42439</v>
       </c>
-      <c r="F36" s="110"/>
-      <c r="G36" s="110">
+      <c r="F37" s="127"/>
+      <c r="G37" s="127">
         <v>42439</v>
       </c>
-      <c r="H36" s="111"/>
-      <c r="I36" s="111" t="s">
+      <c r="H37" s="128"/>
+      <c r="I37" s="128" t="s">
         <v>194</v>
       </c>
-      <c r="J36" s="111"/>
-      <c r="K36" s="111"/>
-      <c r="L36" s="111"/>
-      <c r="M36" s="111"/>
-      <c r="N36" s="111"/>
-      <c r="O36" s="115"/>
-    </row>
-    <row r="37" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="53">
-        <v>15</v>
-      </c>
-      <c r="B37" s="67" t="s">
-        <v>188</v>
-      </c>
-      <c r="C37" s="105">
-        <v>8</v>
-      </c>
-      <c r="D37" s="109"/>
-      <c r="E37" s="110">
+      <c r="J37" s="128"/>
+      <c r="K37" s="128"/>
+      <c r="L37" s="128"/>
+      <c r="M37" s="128"/>
+      <c r="N37" s="128"/>
+      <c r="O37" s="150"/>
+    </row>
+    <row r="38" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="52">
+        <v>16</v>
+      </c>
+      <c r="B38" s="67" t="s">
+        <v>222</v>
+      </c>
+      <c r="C38" s="139">
+        <v>5</v>
+      </c>
+      <c r="D38" s="140"/>
+      <c r="E38" s="127">
         <v>42439</v>
       </c>
-      <c r="F37" s="110"/>
-      <c r="G37" s="110">
-        <v>42439</v>
-      </c>
-      <c r="H37" s="111"/>
-      <c r="I37" s="114" t="s">
-        <v>209</v>
-      </c>
-      <c r="J37" s="111"/>
-      <c r="K37" s="111"/>
-      <c r="L37" s="111"/>
-      <c r="M37" s="111"/>
-      <c r="N37" s="111"/>
-      <c r="O37" s="115"/>
-    </row>
-    <row r="38" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="53">
-        <v>16</v>
-      </c>
-      <c r="B38" s="67" t="s">
-        <v>189</v>
-      </c>
-      <c r="C38" s="105">
-        <v>4</v>
-      </c>
-      <c r="D38" s="109"/>
-      <c r="E38" s="110">
+      <c r="F38" s="127"/>
+      <c r="G38" s="127">
         <v>42440</v>
       </c>
-      <c r="F38" s="110"/>
-      <c r="G38" s="110">
+      <c r="H38" s="128"/>
+      <c r="I38" s="152" t="s">
+        <v>218</v>
+      </c>
+      <c r="J38" s="128"/>
+      <c r="K38" s="128"/>
+      <c r="L38" s="128"/>
+      <c r="M38" s="128"/>
+      <c r="N38" s="128"/>
+      <c r="O38" s="150"/>
+    </row>
+    <row r="39" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="52">
+        <v>17</v>
+      </c>
+      <c r="B39" s="67" t="s">
+        <v>181</v>
+      </c>
+      <c r="C39" s="139">
+        <v>2</v>
+      </c>
+      <c r="D39" s="141"/>
+      <c r="E39" s="125">
         <v>42440</v>
       </c>
-      <c r="H38" s="111"/>
-      <c r="I38" s="114" t="s">
-        <v>211</v>
-      </c>
-      <c r="J38" s="111"/>
-      <c r="K38" s="111"/>
-      <c r="L38" s="111"/>
-      <c r="M38" s="111"/>
-      <c r="N38" s="111"/>
-      <c r="O38" s="115"/>
-    </row>
-    <row r="39" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="99">
-        <v>17</v>
-      </c>
-      <c r="B39" s="100" t="s">
-        <v>195</v>
-      </c>
-      <c r="C39" s="162">
-        <v>10</v>
-      </c>
-      <c r="D39" s="163"/>
-      <c r="E39" s="110">
+      <c r="F39" s="126"/>
+      <c r="G39" s="125">
         <v>42440</v>
       </c>
-      <c r="F39" s="110"/>
-      <c r="G39" s="110">
-        <v>42443</v>
-      </c>
-      <c r="H39" s="111"/>
-      <c r="I39" s="164" t="s">
-        <v>209</v>
-      </c>
-      <c r="J39" s="163"/>
-      <c r="K39" s="163"/>
-      <c r="L39" s="163"/>
-      <c r="M39" s="163"/>
-      <c r="N39" s="163"/>
-      <c r="O39" s="165"/>
+      <c r="H39" s="126"/>
+      <c r="I39" s="134" t="s">
+        <v>192</v>
+      </c>
+      <c r="J39" s="135"/>
+      <c r="K39" s="135"/>
+      <c r="L39" s="135"/>
+      <c r="M39" s="135"/>
+      <c r="N39" s="135"/>
+      <c r="O39" s="136"/>
     </row>
     <row r="40" spans="1:15" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="54">
-        <v>19</v>
-      </c>
-      <c r="B40" s="102" t="s">
-        <v>218</v>
-      </c>
-      <c r="C40" s="179" t="s">
-        <v>207</v>
-      </c>
-      <c r="D40" s="167"/>
-      <c r="E40" s="166"/>
-      <c r="F40" s="167"/>
-      <c r="G40" s="166"/>
-      <c r="H40" s="167"/>
-      <c r="I40" s="168" t="s">
-        <v>219</v>
-      </c>
-      <c r="J40" s="167"/>
-      <c r="K40" s="167"/>
-      <c r="L40" s="167"/>
-      <c r="M40" s="167"/>
-      <c r="N40" s="167"/>
-      <c r="O40" s="169"/>
+        <v>18</v>
+      </c>
+      <c r="B40" s="68" t="s">
+        <v>183</v>
+      </c>
+      <c r="C40" s="142">
+        <v>2</v>
+      </c>
+      <c r="D40" s="143"/>
+      <c r="E40" s="169">
+        <v>42440</v>
+      </c>
+      <c r="F40" s="170"/>
+      <c r="G40" s="169">
+        <v>42440</v>
+      </c>
+      <c r="H40" s="170"/>
+      <c r="I40" s="171" t="s">
+        <v>192</v>
+      </c>
+      <c r="J40" s="172"/>
+      <c r="K40" s="172"/>
+      <c r="L40" s="172"/>
+      <c r="M40" s="172"/>
+      <c r="N40" s="172"/>
+      <c r="O40" s="173"/>
     </row>
     <row r="41" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="69"/>
-      <c r="B41" s="15"/>
-      <c r="C41" s="175">
-        <f>SUM(C29:D40)</f>
-        <v>38</v>
-      </c>
-      <c r="D41" s="175"/>
-      <c r="E41" s="175">
+      <c r="B41" s="71"/>
+      <c r="C41" s="100">
+        <f>SUM(C28:D40)</f>
+        <v>34</v>
+      </c>
+      <c r="D41" s="100"/>
+      <c r="E41" s="100">
         <f>ROUNDUP(C41/(8 + 4), 0)</f>
-        <v>4</v>
-      </c>
-      <c r="F41" s="175"/>
-      <c r="G41" s="15"/>
-      <c r="H41" s="70"/>
-      <c r="I41" s="70"/>
-      <c r="J41" s="70"/>
-      <c r="K41" s="70"/>
-      <c r="L41" s="70"/>
-      <c r="M41" s="70"/>
-      <c r="N41" s="70"/>
-      <c r="O41" s="70"/>
+        <v>3</v>
+      </c>
+      <c r="F41" s="100"/>
+      <c r="G41" s="74"/>
+      <c r="H41" s="74"/>
+      <c r="I41" s="94"/>
+      <c r="J41" s="94"/>
+      <c r="K41" s="94"/>
+      <c r="L41" s="94"/>
+      <c r="M41" s="94"/>
+      <c r="N41" s="94"/>
+      <c r="O41" s="94"/>
     </row>
     <row r="42" spans="1:15" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="69"/>
       <c r="B42" s="15"/>
-      <c r="C42" s="15"/>
-      <c r="D42" s="15"/>
-      <c r="E42" s="15"/>
-      <c r="F42" s="15"/>
+      <c r="C42" s="100"/>
+      <c r="D42" s="100"/>
+      <c r="E42" s="100"/>
+      <c r="F42" s="100"/>
       <c r="G42" s="15"/>
       <c r="H42" s="70"/>
       <c r="I42" s="70"/>
@@ -4809,609 +4619,828 @@
       <c r="N42" s="70"/>
       <c r="O42" s="70"/>
     </row>
-    <row r="43" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="79">
-        <v>18</v>
-      </c>
-      <c r="B43" s="80" t="s">
+    <row r="43" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="64" t="s">
+        <v>190</v>
+      </c>
+      <c r="B43" s="65" t="s">
+        <v>187</v>
+      </c>
+      <c r="C43" s="129" t="s">
+        <v>202</v>
+      </c>
+      <c r="D43" s="130"/>
+      <c r="E43" s="130" t="s">
+        <v>177</v>
+      </c>
+      <c r="F43" s="130"/>
+      <c r="G43" s="130" t="s">
+        <v>178</v>
+      </c>
+      <c r="H43" s="130"/>
+      <c r="I43" s="144" t="s">
+        <v>191</v>
+      </c>
+      <c r="J43" s="130"/>
+      <c r="K43" s="130"/>
+      <c r="L43" s="130"/>
+      <c r="M43" s="130"/>
+      <c r="N43" s="130"/>
+      <c r="O43" s="145"/>
+    </row>
+    <row r="44" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="175">
+        <v>19</v>
+      </c>
+      <c r="B44" s="66" t="s">
+        <v>188</v>
+      </c>
+      <c r="C44" s="179">
+        <v>8</v>
+      </c>
+      <c r="D44" s="147"/>
+      <c r="E44" s="146">
+        <v>42443</v>
+      </c>
+      <c r="F44" s="146"/>
+      <c r="G44" s="146">
+        <v>42443</v>
+      </c>
+      <c r="H44" s="147"/>
+      <c r="I44" s="174" t="s">
+        <v>207</v>
+      </c>
+      <c r="J44" s="147"/>
+      <c r="K44" s="147"/>
+      <c r="L44" s="147"/>
+      <c r="M44" s="147"/>
+      <c r="N44" s="147"/>
+      <c r="O44" s="151"/>
+    </row>
+    <row r="45" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="176">
+        <v>20</v>
+      </c>
+      <c r="B45" s="67" t="s">
+        <v>189</v>
+      </c>
+      <c r="C45" s="141">
+        <v>4</v>
+      </c>
+      <c r="D45" s="128"/>
+      <c r="E45" s="127">
+        <v>42444</v>
+      </c>
+      <c r="F45" s="127"/>
+      <c r="G45" s="127">
+        <v>42444</v>
+      </c>
+      <c r="H45" s="128"/>
+      <c r="I45" s="152" t="s">
+        <v>208</v>
+      </c>
+      <c r="J45" s="128"/>
+      <c r="K45" s="128"/>
+      <c r="L45" s="128"/>
+      <c r="M45" s="128"/>
+      <c r="N45" s="128"/>
+      <c r="O45" s="150"/>
+    </row>
+    <row r="46" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="176">
+        <v>21</v>
+      </c>
+      <c r="B46" s="67" t="s">
+        <v>195</v>
+      </c>
+      <c r="C46" s="140">
+        <v>10</v>
+      </c>
+      <c r="D46" s="128"/>
+      <c r="E46" s="127">
+        <v>42444</v>
+      </c>
+      <c r="F46" s="127"/>
+      <c r="G46" s="127">
+        <v>42445</v>
+      </c>
+      <c r="H46" s="128"/>
+      <c r="I46" s="152" t="s">
+        <v>207</v>
+      </c>
+      <c r="J46" s="128"/>
+      <c r="K46" s="128"/>
+      <c r="L46" s="128"/>
+      <c r="M46" s="128"/>
+      <c r="N46" s="128"/>
+      <c r="O46" s="150"/>
+    </row>
+    <row r="47" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="176">
+        <v>22</v>
+      </c>
+      <c r="B47" s="67" t="s">
+        <v>214</v>
+      </c>
+      <c r="C47" s="140" t="s">
+        <v>205</v>
+      </c>
+      <c r="D47" s="128"/>
+      <c r="E47" s="127"/>
+      <c r="F47" s="128"/>
+      <c r="G47" s="127"/>
+      <c r="H47" s="128"/>
+      <c r="I47" s="152" t="s">
+        <v>224</v>
+      </c>
+      <c r="J47" s="128"/>
+      <c r="K47" s="128"/>
+      <c r="L47" s="128"/>
+      <c r="M47" s="128"/>
+      <c r="N47" s="128"/>
+      <c r="O47" s="150"/>
+    </row>
+    <row r="48" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="176">
+        <v>23</v>
+      </c>
+      <c r="B48" s="67" t="s">
+        <v>223</v>
+      </c>
+      <c r="C48" s="140" t="s">
+        <v>205</v>
+      </c>
+      <c r="D48" s="128"/>
+      <c r="E48" s="127"/>
+      <c r="F48" s="128"/>
+      <c r="G48" s="127"/>
+      <c r="H48" s="128"/>
+      <c r="I48" s="152" t="s">
+        <v>224</v>
+      </c>
+      <c r="J48" s="128"/>
+      <c r="K48" s="128"/>
+      <c r="L48" s="128"/>
+      <c r="M48" s="128"/>
+      <c r="N48" s="128"/>
+      <c r="O48" s="150"/>
+    </row>
+    <row r="49" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="176">
+        <v>24</v>
+      </c>
+      <c r="B49" s="67" t="s">
         <v>197</v>
       </c>
-      <c r="C43" s="180" t="s">
-        <v>206</v>
-      </c>
-      <c r="D43" s="181"/>
-      <c r="E43" s="170"/>
-      <c r="F43" s="171"/>
-      <c r="G43" s="170"/>
-      <c r="H43" s="171"/>
-      <c r="I43" s="171" t="s">
+      <c r="C49" s="140" t="s">
+        <v>205</v>
+      </c>
+      <c r="D49" s="128"/>
+      <c r="E49" s="127"/>
+      <c r="F49" s="128"/>
+      <c r="G49" s="127"/>
+      <c r="H49" s="128"/>
+      <c r="I49" s="152" t="s">
+        <v>224</v>
+      </c>
+      <c r="J49" s="128"/>
+      <c r="K49" s="128"/>
+      <c r="L49" s="128"/>
+      <c r="M49" s="128"/>
+      <c r="N49" s="128"/>
+      <c r="O49" s="150"/>
+    </row>
+    <row r="50" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="176">
+        <v>25</v>
+      </c>
+      <c r="B50" s="67" t="s">
+        <v>198</v>
+      </c>
+      <c r="C50" s="135" t="s">
+        <v>204</v>
+      </c>
+      <c r="D50" s="140"/>
+      <c r="E50" s="125"/>
+      <c r="F50" s="126"/>
+      <c r="G50" s="125"/>
+      <c r="H50" s="126"/>
+      <c r="I50" s="152" t="s">
+        <v>224</v>
+      </c>
+      <c r="J50" s="128"/>
+      <c r="K50" s="128"/>
+      <c r="L50" s="128"/>
+      <c r="M50" s="128"/>
+      <c r="N50" s="128"/>
+      <c r="O50" s="150"/>
+    </row>
+    <row r="51" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="176">
+        <v>26</v>
+      </c>
+      <c r="B51" s="67" t="s">
+        <v>225</v>
+      </c>
+      <c r="C51" s="140" t="s">
+        <v>204</v>
+      </c>
+      <c r="D51" s="128"/>
+      <c r="E51" s="127"/>
+      <c r="F51" s="128"/>
+      <c r="G51" s="127"/>
+      <c r="H51" s="128"/>
+      <c r="I51" s="152" t="s">
+        <v>224</v>
+      </c>
+      <c r="J51" s="128"/>
+      <c r="K51" s="128"/>
+      <c r="L51" s="128"/>
+      <c r="M51" s="128"/>
+      <c r="N51" s="128"/>
+      <c r="O51" s="150"/>
+    </row>
+    <row r="52" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="176">
+        <v>27</v>
+      </c>
+      <c r="B52" s="67" t="s">
+        <v>199</v>
+      </c>
+      <c r="C52" s="140" t="s">
+        <v>204</v>
+      </c>
+      <c r="D52" s="128"/>
+      <c r="E52" s="127"/>
+      <c r="F52" s="128"/>
+      <c r="G52" s="127"/>
+      <c r="H52" s="128"/>
+      <c r="I52" s="152" t="s">
+        <v>224</v>
+      </c>
+      <c r="J52" s="128"/>
+      <c r="K52" s="128"/>
+      <c r="L52" s="128"/>
+      <c r="M52" s="128"/>
+      <c r="N52" s="128"/>
+      <c r="O52" s="150"/>
+    </row>
+    <row r="53" spans="1:15" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="177">
+        <v>28</v>
+      </c>
+      <c r="B53" s="68" t="s">
+        <v>200</v>
+      </c>
+      <c r="C53" s="180" t="s">
+        <v>204</v>
+      </c>
+      <c r="D53" s="131"/>
+      <c r="E53" s="133"/>
+      <c r="F53" s="131"/>
+      <c r="G53" s="133"/>
+      <c r="H53" s="131"/>
+      <c r="I53" s="178" t="s">
+        <v>224</v>
+      </c>
+      <c r="J53" s="131"/>
+      <c r="K53" s="131"/>
+      <c r="L53" s="131"/>
+      <c r="M53" s="131"/>
+      <c r="N53" s="131"/>
+      <c r="O53" s="132"/>
+    </row>
+    <row r="54" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="69"/>
+      <c r="B54" s="71"/>
+      <c r="C54" s="94"/>
+      <c r="D54" s="94"/>
+      <c r="E54" s="74"/>
+      <c r="F54" s="94"/>
+      <c r="G54" s="74"/>
+      <c r="H54" s="94"/>
+      <c r="I54" s="94"/>
+      <c r="J54" s="94"/>
+      <c r="K54" s="94"/>
+      <c r="L54" s="94"/>
+      <c r="M54" s="94"/>
+      <c r="N54" s="94"/>
+      <c r="O54" s="94"/>
+    </row>
+    <row r="55" spans="1:15" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="69"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="15"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="70"/>
+      <c r="I55" s="70"/>
+      <c r="J55" s="70"/>
+      <c r="K55" s="70"/>
+      <c r="L55" s="70"/>
+      <c r="M55" s="70"/>
+      <c r="N55" s="70"/>
+      <c r="O55" s="70"/>
+    </row>
+    <row r="56" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="76"/>
+      <c r="B56" s="77" t="s">
+        <v>196</v>
+      </c>
+      <c r="C56" s="157">
+        <v>5</v>
+      </c>
+      <c r="D56" s="157"/>
+      <c r="E56" s="158">
+        <v>42460</v>
+      </c>
+      <c r="F56" s="157"/>
+      <c r="G56" s="158">
+        <v>42465</v>
+      </c>
+      <c r="H56" s="157"/>
+      <c r="I56" s="90"/>
+      <c r="J56" s="90"/>
+      <c r="K56" s="90"/>
+      <c r="L56" s="90"/>
+      <c r="M56" s="90"/>
+      <c r="N56" s="90"/>
+      <c r="O56" s="78"/>
+    </row>
+    <row r="57" spans="1:15" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="79"/>
+      <c r="B57" s="80" t="s">
         <v>201</v>
       </c>
-      <c r="J43" s="171"/>
-      <c r="K43" s="171"/>
-      <c r="L43" s="171"/>
-      <c r="M43" s="171"/>
-      <c r="N43" s="171"/>
-      <c r="O43" s="172"/>
-    </row>
-    <row r="44" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="53">
-        <v>19</v>
-      </c>
-      <c r="B44" s="74" t="s">
-        <v>198</v>
-      </c>
-      <c r="C44" s="182" t="s">
-        <v>206</v>
-      </c>
-      <c r="D44" s="112"/>
-      <c r="E44" s="125"/>
-      <c r="F44" s="113"/>
-      <c r="G44" s="125"/>
-      <c r="H44" s="113"/>
-      <c r="I44" s="113" t="s">
-        <v>201</v>
-      </c>
-      <c r="J44" s="113"/>
-      <c r="K44" s="113"/>
-      <c r="L44" s="113"/>
-      <c r="M44" s="113"/>
-      <c r="N44" s="113"/>
-      <c r="O44" s="127"/>
-    </row>
-    <row r="45" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="53">
-        <v>20</v>
-      </c>
-      <c r="B45" s="74" t="s">
-        <v>199</v>
-      </c>
-      <c r="C45" s="182" t="s">
-        <v>206</v>
-      </c>
-      <c r="D45" s="112"/>
-      <c r="E45" s="125"/>
-      <c r="F45" s="113"/>
-      <c r="G45" s="125"/>
-      <c r="H45" s="113"/>
-      <c r="I45" s="113" t="s">
-        <v>201</v>
-      </c>
-      <c r="J45" s="113"/>
-      <c r="K45" s="113"/>
-      <c r="L45" s="113"/>
-      <c r="M45" s="113"/>
-      <c r="N45" s="113"/>
-      <c r="O45" s="127"/>
-    </row>
-    <row r="46" spans="1:15" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="54">
-        <v>21</v>
-      </c>
-      <c r="B46" s="81" t="s">
-        <v>200</v>
-      </c>
-      <c r="C46" s="183" t="s">
-        <v>206</v>
-      </c>
-      <c r="D46" s="179"/>
-      <c r="E46" s="166"/>
-      <c r="F46" s="167"/>
-      <c r="G46" s="166"/>
-      <c r="H46" s="167"/>
-      <c r="I46" s="167" t="s">
-        <v>201</v>
-      </c>
-      <c r="J46" s="167"/>
-      <c r="K46" s="167"/>
-      <c r="L46" s="167"/>
-      <c r="M46" s="167"/>
-      <c r="N46" s="167"/>
-      <c r="O46" s="169"/>
-    </row>
-    <row r="47" spans="1:15" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="69"/>
-      <c r="B47" s="15"/>
-      <c r="C47" s="15"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="15"/>
-      <c r="F47" s="15"/>
-      <c r="G47" s="15"/>
-      <c r="H47" s="70"/>
-      <c r="I47" s="70"/>
-      <c r="J47" s="70"/>
-      <c r="K47" s="70"/>
-      <c r="L47" s="70"/>
-      <c r="M47" s="70"/>
-      <c r="N47" s="70"/>
-      <c r="O47" s="70"/>
-    </row>
-    <row r="48" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="82"/>
-      <c r="B48" s="83" t="s">
-        <v>196</v>
-      </c>
-      <c r="C48" s="123">
+      <c r="C57" s="160" t="s">
+        <v>204</v>
+      </c>
+      <c r="D57" s="160"/>
+      <c r="E57" s="161">
+        <v>42440</v>
+      </c>
+      <c r="F57" s="161"/>
+      <c r="G57" s="161">
+        <v>42453</v>
+      </c>
+      <c r="H57" s="161"/>
+      <c r="I57" s="91"/>
+      <c r="J57" s="91"/>
+      <c r="K57" s="91"/>
+      <c r="L57" s="91"/>
+      <c r="M57" s="91"/>
+      <c r="N57" s="91"/>
+      <c r="O57" s="81"/>
+    </row>
+    <row r="58" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="69"/>
+      <c r="B58" s="15"/>
+      <c r="C58" s="15"/>
+      <c r="D58" s="15"/>
+      <c r="E58" s="15"/>
+      <c r="F58" s="15"/>
+      <c r="G58" s="15"/>
+      <c r="H58" s="70"/>
+      <c r="I58" s="70"/>
+      <c r="J58" s="70"/>
+      <c r="K58" s="70"/>
+      <c r="L58" s="70"/>
+      <c r="M58" s="70"/>
+      <c r="N58" s="70"/>
+      <c r="O58" s="70"/>
+    </row>
+    <row r="59" spans="1:15" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="69"/>
+      <c r="B59" s="15"/>
+      <c r="C59" s="15"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="15"/>
+      <c r="F59" s="15"/>
+      <c r="G59" s="15"/>
+      <c r="H59" s="70"/>
+      <c r="I59" s="70"/>
+      <c r="J59" s="70"/>
+      <c r="K59" s="70"/>
+      <c r="L59" s="70"/>
+      <c r="M59" s="70"/>
+      <c r="N59" s="70"/>
+      <c r="O59" s="70"/>
+    </row>
+    <row r="60" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="104" t="s">
+        <v>50</v>
+      </c>
+      <c r="B60" s="107" t="s">
+        <v>37</v>
+      </c>
+      <c r="C60" s="110" t="s">
+        <v>38</v>
+      </c>
+      <c r="D60" s="113" t="s">
+        <v>166</v>
+      </c>
+      <c r="E60" s="113" t="s">
+        <v>167</v>
+      </c>
+      <c r="F60" s="116" t="s">
+        <v>54</v>
+      </c>
+      <c r="G60" s="116" t="s">
+        <v>169</v>
+      </c>
+      <c r="H60" s="119" t="s">
+        <v>56</v>
+      </c>
+      <c r="I60" s="120"/>
+      <c r="J60" s="120"/>
+      <c r="K60" s="120"/>
+      <c r="L60" s="120"/>
+      <c r="M60" s="120"/>
+      <c r="N60" s="120"/>
+      <c r="O60" s="121"/>
+    </row>
+    <row r="61" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="105"/>
+      <c r="B61" s="108"/>
+      <c r="C61" s="111"/>
+      <c r="D61" s="114"/>
+      <c r="E61" s="114"/>
+      <c r="F61" s="117"/>
+      <c r="G61" s="117"/>
+      <c r="H61" s="60">
+        <v>1</v>
+      </c>
+      <c r="I61" s="61">
+        <v>2</v>
+      </c>
+      <c r="J61" s="60">
+        <v>3</v>
+      </c>
+      <c r="K61" s="60">
+        <v>4</v>
+      </c>
+      <c r="L61" s="60">
         <v>5</v>
       </c>
-      <c r="D48" s="123"/>
-      <c r="E48" s="124">
-        <v>42460</v>
-      </c>
-      <c r="F48" s="123"/>
-      <c r="G48" s="124">
-        <v>42465</v>
-      </c>
-      <c r="H48" s="123"/>
-      <c r="I48" s="96"/>
-      <c r="J48" s="96"/>
-      <c r="K48" s="96"/>
-      <c r="L48" s="96"/>
-      <c r="M48" s="96"/>
-      <c r="N48" s="96"/>
-      <c r="O48" s="84"/>
-    </row>
-    <row r="49" spans="1:15" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="85"/>
-      <c r="B49" s="86" t="s">
-        <v>203</v>
-      </c>
-      <c r="C49" s="103" t="s">
-        <v>206</v>
-      </c>
-      <c r="D49" s="103"/>
-      <c r="E49" s="104">
-        <v>42440</v>
-      </c>
-      <c r="F49" s="104"/>
-      <c r="G49" s="104">
-        <v>42453</v>
-      </c>
-      <c r="H49" s="104"/>
-      <c r="I49" s="97"/>
-      <c r="J49" s="97"/>
-      <c r="K49" s="97"/>
-      <c r="L49" s="97"/>
-      <c r="M49" s="97"/>
-      <c r="N49" s="97"/>
-      <c r="O49" s="87"/>
-    </row>
-    <row r="50" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="69"/>
-      <c r="B50" s="15"/>
-      <c r="C50" s="15"/>
-      <c r="D50" s="15"/>
-      <c r="E50" s="15"/>
-      <c r="F50" s="15"/>
-      <c r="G50" s="15"/>
-      <c r="H50" s="70"/>
-      <c r="I50" s="70"/>
-      <c r="J50" s="70"/>
-      <c r="K50" s="70"/>
-      <c r="L50" s="70"/>
-      <c r="M50" s="70"/>
-      <c r="N50" s="70"/>
-      <c r="O50" s="70"/>
-    </row>
-    <row r="51" spans="1:15" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="69"/>
-      <c r="B51" s="15"/>
-      <c r="C51" s="15"/>
-      <c r="D51" s="15"/>
-      <c r="E51" s="15"/>
-      <c r="F51" s="15"/>
-      <c r="G51" s="15"/>
-      <c r="H51" s="70"/>
-      <c r="I51" s="70"/>
-      <c r="J51" s="70"/>
-      <c r="K51" s="70"/>
-      <c r="L51" s="70"/>
-      <c r="M51" s="70"/>
-      <c r="N51" s="70"/>
-      <c r="O51" s="70"/>
-    </row>
-    <row r="52" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="142" t="s">
-        <v>50</v>
-      </c>
-      <c r="B52" s="148" t="s">
-        <v>37</v>
-      </c>
-      <c r="C52" s="136" t="s">
-        <v>38</v>
-      </c>
-      <c r="D52" s="151" t="s">
-        <v>166</v>
-      </c>
-      <c r="E52" s="151" t="s">
-        <v>167</v>
-      </c>
-      <c r="F52" s="139" t="s">
-        <v>54</v>
-      </c>
-      <c r="G52" s="139" t="s">
-        <v>169</v>
-      </c>
-      <c r="H52" s="145" t="s">
-        <v>56</v>
-      </c>
-      <c r="I52" s="146"/>
-      <c r="J52" s="146"/>
-      <c r="K52" s="146"/>
-      <c r="L52" s="146"/>
-      <c r="M52" s="146"/>
-      <c r="N52" s="146"/>
-      <c r="O52" s="147"/>
-    </row>
-    <row r="53" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="143"/>
-      <c r="B53" s="149"/>
-      <c r="C53" s="137"/>
-      <c r="D53" s="152"/>
-      <c r="E53" s="152"/>
-      <c r="F53" s="140"/>
-      <c r="G53" s="140"/>
-      <c r="H53" s="60">
+      <c r="M61" s="60">
+        <v>6</v>
+      </c>
+      <c r="N61" s="63">
+        <v>7</v>
+      </c>
+      <c r="O61" s="29">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="106"/>
+      <c r="B62" s="109"/>
+      <c r="C62" s="112"/>
+      <c r="D62" s="115"/>
+      <c r="E62" s="115"/>
+      <c r="F62" s="118"/>
+      <c r="G62" s="118"/>
+      <c r="H62" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="I62" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="J62" s="49" t="s">
+        <v>171</v>
+      </c>
+      <c r="K62" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="L62" s="50" t="s">
+        <v>173</v>
+      </c>
+      <c r="M62" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="N62" s="50" t="s">
+        <v>47</v>
+      </c>
+      <c r="O62" s="62" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="51">
         <v>1</v>
       </c>
-      <c r="I53" s="61">
+      <c r="B63" s="55" t="s">
+        <v>175</v>
+      </c>
+      <c r="C63" s="44" t="s">
+        <v>174</v>
+      </c>
+      <c r="D63" s="44" t="s">
+        <v>174</v>
+      </c>
+      <c r="E63" s="44" t="s">
+        <v>174</v>
+      </c>
+      <c r="F63" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="G63" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="H63" s="87" t="s">
+        <v>43</v>
+      </c>
+      <c r="I63" s="87" t="s">
+        <v>43</v>
+      </c>
+      <c r="J63" s="46" t="s">
+        <v>172</v>
+      </c>
+      <c r="K63" s="85" t="s">
+        <v>53</v>
+      </c>
+      <c r="L63" s="85" t="s">
+        <v>43</v>
+      </c>
+      <c r="M63" s="96" t="s">
+        <v>43</v>
+      </c>
+      <c r="N63" s="85" t="s">
+        <v>43</v>
+      </c>
+      <c r="O63" s="48" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="52">
         <v>2</v>
       </c>
-      <c r="J53" s="60">
+      <c r="B64" s="56" t="s">
+        <v>51</v>
+      </c>
+      <c r="C64" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="D64" s="30"/>
+      <c r="E64" s="30"/>
+      <c r="F64" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="G64" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="H64" s="88" t="s">
+        <v>43</v>
+      </c>
+      <c r="I64" s="86" t="s">
+        <v>43</v>
+      </c>
+      <c r="J64" s="32" t="s">
+        <v>172</v>
+      </c>
+      <c r="K64" s="86" t="s">
+        <v>43</v>
+      </c>
+      <c r="L64" s="86" t="s">
+        <v>43</v>
+      </c>
+      <c r="M64" s="97" t="s">
+        <v>43</v>
+      </c>
+      <c r="N64" s="86" t="s">
+        <v>43</v>
+      </c>
+      <c r="O64" s="89" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="52">
         <v>3</v>
       </c>
-      <c r="K53" s="60">
+      <c r="B65" s="56" t="s">
+        <v>39</v>
+      </c>
+      <c r="C65" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="D65" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="E65" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="F65" s="35"/>
+      <c r="G65" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="H65" s="32"/>
+      <c r="I65" s="32"/>
+      <c r="J65" s="32"/>
+      <c r="K65" s="32"/>
+      <c r="L65" s="32"/>
+      <c r="M65" s="33"/>
+      <c r="N65" s="32"/>
+      <c r="O65" s="34"/>
+    </row>
+    <row r="66" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="52">
         <v>4</v>
       </c>
-      <c r="L53" s="60">
+      <c r="B66" s="56" t="s">
+        <v>52</v>
+      </c>
+      <c r="C66" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="D66" s="30"/>
+      <c r="E66" s="30"/>
+      <c r="F66" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="G66" s="36" t="s">
+        <v>170</v>
+      </c>
+      <c r="H66" s="95" t="s">
+        <v>170</v>
+      </c>
+      <c r="I66" s="88" t="s">
+        <v>43</v>
+      </c>
+      <c r="J66" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="K66" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="L66" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="M66" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="N66" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="O66" s="34" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="52">
         <v>5</v>
       </c>
-      <c r="M53" s="60">
+      <c r="B67" s="59" t="s">
+        <v>40</v>
+      </c>
+      <c r="C67" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="D67" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="E67" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="F67" s="35"/>
+      <c r="G67" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="H67" s="32"/>
+      <c r="I67" s="32"/>
+      <c r="J67" s="32"/>
+      <c r="K67" s="32"/>
+      <c r="L67" s="32"/>
+      <c r="M67" s="33"/>
+      <c r="N67" s="32"/>
+      <c r="O67" s="34"/>
+    </row>
+    <row r="68" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="53">
         <v>6</v>
       </c>
-      <c r="N53" s="63">
+      <c r="B68" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="C68" s="44" t="s">
+        <v>174</v>
+      </c>
+      <c r="D68" s="44" t="s">
+        <v>174</v>
+      </c>
+      <c r="E68" s="44"/>
+      <c r="F68" s="58"/>
+      <c r="G68" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="H68" s="46"/>
+      <c r="I68" s="46"/>
+      <c r="J68" s="46"/>
+      <c r="K68" s="46"/>
+      <c r="L68" s="46"/>
+      <c r="M68" s="47"/>
+      <c r="N68" s="46"/>
+      <c r="O68" s="48"/>
+    </row>
+    <row r="69" spans="1:15" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="54">
         <v>7</v>
       </c>
-      <c r="O53" s="29">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="144"/>
-      <c r="B54" s="150"/>
-      <c r="C54" s="138"/>
-      <c r="D54" s="153"/>
-      <c r="E54" s="153"/>
-      <c r="F54" s="141"/>
-      <c r="G54" s="141"/>
-      <c r="H54" s="49" t="s">
-        <v>45</v>
-      </c>
-      <c r="I54" s="49" t="s">
-        <v>44</v>
-      </c>
-      <c r="J54" s="49" t="s">
-        <v>171</v>
-      </c>
-      <c r="K54" s="49" t="s">
-        <v>49</v>
-      </c>
-      <c r="L54" s="50" t="s">
-        <v>173</v>
-      </c>
-      <c r="M54" s="50" t="s">
-        <v>46</v>
-      </c>
-      <c r="N54" s="50" t="s">
-        <v>47</v>
-      </c>
-      <c r="O54" s="62" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="51">
-        <v>1</v>
-      </c>
-      <c r="B55" s="55" t="s">
-        <v>175</v>
-      </c>
-      <c r="C55" s="44" t="s">
+      <c r="B69" s="57" t="s">
+        <v>42</v>
+      </c>
+      <c r="C69" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="D55" s="44" t="s">
+      <c r="D69" s="38"/>
+      <c r="E69" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="E55" s="44" t="s">
-        <v>174</v>
-      </c>
-      <c r="F55" s="45" t="s">
-        <v>55</v>
-      </c>
-      <c r="G55" s="45" t="s">
-        <v>55</v>
-      </c>
-      <c r="H55" s="93" t="s">
-        <v>43</v>
-      </c>
-      <c r="I55" s="93" t="s">
-        <v>43</v>
-      </c>
-      <c r="J55" s="46" t="s">
-        <v>172</v>
-      </c>
-      <c r="K55" s="91" t="s">
-        <v>53</v>
-      </c>
-      <c r="L55" s="91" t="s">
-        <v>43</v>
-      </c>
-      <c r="M55" s="191" t="s">
-        <v>43</v>
-      </c>
-      <c r="N55" s="91" t="s">
-        <v>43</v>
-      </c>
-      <c r="O55" s="48" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="52">
-        <v>2</v>
-      </c>
-      <c r="B56" s="56" t="s">
-        <v>51</v>
-      </c>
-      <c r="C56" s="30" t="s">
-        <v>174</v>
-      </c>
-      <c r="D56" s="30"/>
-      <c r="E56" s="30"/>
-      <c r="F56" s="30" t="s">
-        <v>174</v>
-      </c>
-      <c r="G56" s="30" t="s">
-        <v>174</v>
-      </c>
-      <c r="H56" s="94" t="s">
-        <v>43</v>
-      </c>
-      <c r="I56" s="92" t="s">
-        <v>43</v>
-      </c>
-      <c r="J56" s="32" t="s">
-        <v>172</v>
-      </c>
-      <c r="K56" s="92" t="s">
-        <v>43</v>
-      </c>
-      <c r="L56" s="92" t="s">
-        <v>43</v>
-      </c>
-      <c r="M56" s="192" t="s">
-        <v>43</v>
-      </c>
-      <c r="N56" s="92" t="s">
-        <v>43</v>
-      </c>
-      <c r="O56" s="95" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="52">
-        <v>3</v>
-      </c>
-      <c r="B57" s="56" t="s">
-        <v>39</v>
-      </c>
-      <c r="C57" s="30" t="s">
-        <v>174</v>
-      </c>
-      <c r="D57" s="30" t="s">
-        <v>174</v>
-      </c>
-      <c r="E57" s="30" t="s">
-        <v>174</v>
-      </c>
-      <c r="F57" s="35"/>
-      <c r="G57" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="H57" s="32"/>
-      <c r="I57" s="32"/>
-      <c r="J57" s="32"/>
-      <c r="K57" s="32"/>
-      <c r="L57" s="32"/>
-      <c r="M57" s="33"/>
-      <c r="N57" s="32"/>
-      <c r="O57" s="34"/>
-    </row>
-    <row r="58" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="52">
-        <v>4</v>
-      </c>
-      <c r="B58" s="56" t="s">
-        <v>52</v>
-      </c>
-      <c r="C58" s="30" t="s">
-        <v>174</v>
-      </c>
-      <c r="D58" s="30"/>
-      <c r="E58" s="30"/>
-      <c r="F58" s="30" t="s">
-        <v>174</v>
-      </c>
-      <c r="G58" s="36" t="s">
-        <v>170</v>
-      </c>
-      <c r="H58" s="190" t="s">
-        <v>170</v>
-      </c>
-      <c r="I58" s="94" t="s">
-        <v>43</v>
-      </c>
-      <c r="J58" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="K58" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="L58" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="M58" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="N58" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="O58" s="34" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="52">
-        <v>5</v>
-      </c>
-      <c r="B59" s="59" t="s">
-        <v>40</v>
-      </c>
-      <c r="C59" s="30" t="s">
-        <v>174</v>
-      </c>
-      <c r="D59" s="30" t="s">
-        <v>174</v>
-      </c>
-      <c r="E59" s="30" t="s">
-        <v>174</v>
-      </c>
-      <c r="F59" s="35"/>
-      <c r="G59" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="H59" s="32"/>
-      <c r="I59" s="32"/>
-      <c r="J59" s="32"/>
-      <c r="K59" s="32"/>
-      <c r="L59" s="32"/>
-      <c r="M59" s="33"/>
-      <c r="N59" s="32"/>
-      <c r="O59" s="34"/>
-    </row>
-    <row r="60" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="53">
-        <v>6</v>
-      </c>
-      <c r="B60" s="55" t="s">
-        <v>41</v>
-      </c>
-      <c r="C60" s="44" t="s">
-        <v>174</v>
-      </c>
-      <c r="D60" s="44" t="s">
-        <v>174</v>
-      </c>
-      <c r="E60" s="44"/>
-      <c r="F60" s="58"/>
-      <c r="G60" s="45" t="s">
-        <v>55</v>
-      </c>
-      <c r="H60" s="46"/>
-      <c r="I60" s="46"/>
-      <c r="J60" s="46"/>
-      <c r="K60" s="46"/>
-      <c r="L60" s="46"/>
-      <c r="M60" s="47"/>
-      <c r="N60" s="46"/>
-      <c r="O60" s="48"/>
-    </row>
-    <row r="61" spans="1:15" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="54">
-        <v>7</v>
-      </c>
-      <c r="B61" s="57" t="s">
-        <v>42</v>
-      </c>
-      <c r="C61" s="38" t="s">
-        <v>174</v>
-      </c>
-      <c r="D61" s="38"/>
-      <c r="E61" s="38" t="s">
-        <v>174</v>
-      </c>
-      <c r="F61" s="39"/>
-      <c r="G61" s="40" t="s">
+      <c r="F69" s="39"/>
+      <c r="G69" s="40" t="s">
         <v>168</v>
       </c>
-      <c r="H61" s="41"/>
-      <c r="I61" s="41"/>
-      <c r="J61" s="41"/>
-      <c r="K61" s="41"/>
-      <c r="L61" s="41"/>
-      <c r="M61" s="42"/>
-      <c r="N61" s="41"/>
-      <c r="O61" s="43"/>
+      <c r="H69" s="41"/>
+      <c r="I69" s="41"/>
+      <c r="J69" s="41"/>
+      <c r="K69" s="41"/>
+      <c r="L69" s="41"/>
+      <c r="M69" s="42"/>
+      <c r="N69" s="41"/>
+      <c r="O69" s="43"/>
     </row>
   </sheetData>
-  <mergeCells count="124">
-    <mergeCell ref="C17:D17"/>
+  <mergeCells count="154">
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="I47:O47"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="I49:O49"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="I48:O48"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="I44:O44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="I45:O45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="I46:O46"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="G38:H38"/>
     <mergeCell ref="C41:D41"/>
     <mergeCell ref="E41:F41"/>
-    <mergeCell ref="I17:O17"/>
-    <mergeCell ref="A52:A54"/>
-    <mergeCell ref="B52:B54"/>
-    <mergeCell ref="C52:C54"/>
-    <mergeCell ref="D52:D54"/>
-    <mergeCell ref="E52:E54"/>
-    <mergeCell ref="F52:F54"/>
-    <mergeCell ref="G52:G54"/>
-    <mergeCell ref="H52:O52"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="I44:O44"/>
-    <mergeCell ref="I45:O45"/>
-    <mergeCell ref="I46:O46"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="I40:O40"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="I43:O43"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="I33:O33"/>
+    <mergeCell ref="I34:O34"/>
+    <mergeCell ref="I36:O36"/>
+    <mergeCell ref="I38:O38"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:O32"/>
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="E39:F39"/>
     <mergeCell ref="G39:H39"/>
     <mergeCell ref="I39:O39"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="I25:O25"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="I30:O30"/>
-    <mergeCell ref="I31:O31"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="I19:O19"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="I40:O40"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="I35:O35"/>
+    <mergeCell ref="C37:D37"/>
     <mergeCell ref="C2:C4"/>
     <mergeCell ref="F2:F4"/>
     <mergeCell ref="A2:A4"/>
@@ -5422,64 +5451,83 @@
     <mergeCell ref="G2:G4"/>
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="G21:H21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:H22"/>
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="G19:H19"/>
     <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I20:O20"/>
+    <mergeCell ref="I21:O21"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="I19:O19"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:H22"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="I22:O22"/>
-    <mergeCell ref="I20:O20"/>
-    <mergeCell ref="I21:O21"/>
     <mergeCell ref="I24:O24"/>
-    <mergeCell ref="I38:O38"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="E23:F23"/>
     <mergeCell ref="G23:H23"/>
     <mergeCell ref="I23:O23"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="I33:O33"/>
-    <mergeCell ref="I34:O34"/>
-    <mergeCell ref="I35:O35"/>
-    <mergeCell ref="I36:O36"/>
-    <mergeCell ref="I37:O37"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:O32"/>
     <mergeCell ref="G28:H28"/>
     <mergeCell ref="I28:O28"/>
     <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="I43:O43"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="I25:O25"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I30:O30"/>
+    <mergeCell ref="I31:O31"/>
+    <mergeCell ref="E31:F31"/>
     <mergeCell ref="E29:F29"/>
     <mergeCell ref="G29:H29"/>
     <mergeCell ref="I29:O29"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="C37:D37"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="G37:H37"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="I37:O37"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="G53:H53"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="I50:O50"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="I17:O17"/>
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="B60:B62"/>
+    <mergeCell ref="C60:C62"/>
+    <mergeCell ref="D60:D62"/>
+    <mergeCell ref="E60:E62"/>
+    <mergeCell ref="F60:F62"/>
+    <mergeCell ref="G60:G62"/>
+    <mergeCell ref="H60:O60"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="I51:O51"/>
+    <mergeCell ref="I52:O52"/>
+    <mergeCell ref="I53:O53"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="E52:F52"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5520,10 +5568,10 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="184" t="s">
+      <c r="A3" s="162" t="s">
         <v>109</v>
       </c>
-      <c r="B3" s="184" t="s">
+      <c r="B3" s="162" t="s">
         <v>110</v>
       </c>
       <c r="C3" s="28" t="s">
@@ -5534,8 +5582,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="184"/>
-      <c r="B4" s="184"/>
+      <c r="A4" s="162"/>
+      <c r="B4" s="162"/>
       <c r="C4" s="28" t="s">
         <v>118</v>
       </c>
@@ -5544,8 +5592,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="184"/>
-      <c r="B5" s="184"/>
+      <c r="A5" s="162"/>
+      <c r="B5" s="162"/>
       <c r="C5" s="28" t="s">
         <v>119</v>
       </c>
@@ -5554,8 +5602,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="184"/>
-      <c r="B6" s="184"/>
+      <c r="A6" s="162"/>
+      <c r="B6" s="162"/>
       <c r="C6" s="28" t="s">
         <v>120</v>
       </c>
@@ -5564,8 +5612,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="184"/>
-      <c r="B7" s="184" t="s">
+      <c r="A7" s="162"/>
+      <c r="B7" s="162" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="28" t="s">
@@ -5576,8 +5624,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="184"/>
-      <c r="B8" s="184"/>
+      <c r="A8" s="162"/>
+      <c r="B8" s="162"/>
       <c r="C8" s="28" t="s">
         <v>122</v>
       </c>
@@ -5586,8 +5634,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="184"/>
-      <c r="B9" s="184"/>
+      <c r="A9" s="162"/>
+      <c r="B9" s="162"/>
       <c r="C9" s="28" t="s">
         <v>123</v>
       </c>
@@ -5596,8 +5644,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="184"/>
-      <c r="B10" s="184"/>
+      <c r="A10" s="162"/>
+      <c r="B10" s="162"/>
       <c r="C10" s="28" t="s">
         <v>124</v>
       </c>
@@ -5606,8 +5654,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A11" s="184"/>
-      <c r="B11" s="184" t="s">
+      <c r="A11" s="162"/>
+      <c r="B11" s="162" t="s">
         <v>111</v>
       </c>
       <c r="C11" s="28" t="s">
@@ -5618,8 +5666,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="184"/>
-      <c r="B12" s="184"/>
+      <c r="A12" s="162"/>
+      <c r="B12" s="162"/>
       <c r="C12" s="28" t="s">
         <v>126</v>
       </c>
@@ -5628,8 +5676,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A13" s="184"/>
-      <c r="B13" s="184" t="s">
+      <c r="A13" s="162"/>
+      <c r="B13" s="162" t="s">
         <v>112</v>
       </c>
       <c r="C13" s="28" t="s">
@@ -5640,8 +5688,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="184"/>
-      <c r="B14" s="184"/>
+      <c r="A14" s="162"/>
+      <c r="B14" s="162"/>
       <c r="C14" s="28" t="s">
         <v>128</v>
       </c>
@@ -5650,8 +5698,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="184"/>
-      <c r="B15" s="184" t="s">
+      <c r="A15" s="162"/>
+      <c r="B15" s="162" t="s">
         <v>113</v>
       </c>
       <c r="C15" s="28" t="s">
@@ -5662,8 +5710,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="184"/>
-      <c r="B16" s="184"/>
+      <c r="A16" s="162"/>
+      <c r="B16" s="162"/>
       <c r="C16" s="28" t="s">
         <v>142</v>
       </c>
@@ -5672,8 +5720,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="184"/>
-      <c r="B17" s="184" t="s">
+      <c r="A17" s="162"/>
+      <c r="B17" s="162" t="s">
         <v>114</v>
       </c>
       <c r="C17" s="28" t="s">
@@ -5684,8 +5732,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="184"/>
-      <c r="B18" s="184"/>
+      <c r="A18" s="162"/>
+      <c r="B18" s="162"/>
       <c r="C18" s="28" t="s">
         <v>139</v>
       </c>
@@ -5694,8 +5742,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="184"/>
-      <c r="B19" s="184"/>
+      <c r="A19" s="162"/>
+      <c r="B19" s="162"/>
       <c r="C19" s="28" t="s">
         <v>138</v>
       </c>
@@ -5704,8 +5752,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A20" s="184"/>
-      <c r="B20" s="184" t="s">
+      <c r="A20" s="162"/>
+      <c r="B20" s="162" t="s">
         <v>115</v>
       </c>
       <c r="C20" s="28" t="s">
@@ -5716,8 +5764,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="184"/>
-      <c r="B21" s="184"/>
+      <c r="A21" s="162"/>
+      <c r="B21" s="162"/>
       <c r="C21" s="28" t="s">
         <v>136</v>
       </c>
@@ -5726,8 +5774,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="184"/>
-      <c r="B22" s="184"/>
+      <c r="A22" s="162"/>
+      <c r="B22" s="162"/>
       <c r="C22" s="28" t="s">
         <v>135</v>
       </c>
@@ -5736,8 +5784,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A23" s="184"/>
-      <c r="B23" s="184"/>
+      <c r="A23" s="162"/>
+      <c r="B23" s="162"/>
       <c r="C23" s="28" t="s">
         <v>134</v>
       </c>
@@ -5746,8 +5794,8 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A24" s="184"/>
-      <c r="B24" s="184"/>
+      <c r="A24" s="162"/>
+      <c r="B24" s="162"/>
       <c r="C24" s="28" t="s">
         <v>133</v>
       </c>
@@ -5756,8 +5804,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="184"/>
-      <c r="B25" s="184"/>
+      <c r="A25" s="162"/>
+      <c r="B25" s="162"/>
       <c r="C25" s="28" t="s">
         <v>132</v>
       </c>
@@ -5766,8 +5814,8 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A26" s="184"/>
-      <c r="B26" s="184" t="s">
+      <c r="A26" s="162"/>
+      <c r="B26" s="162" t="s">
         <v>116</v>
       </c>
       <c r="C26" s="28" t="s">
@@ -5778,8 +5826,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="184"/>
-      <c r="B27" s="184"/>
+      <c r="A27" s="162"/>
+      <c r="B27" s="162"/>
       <c r="C27" s="28" t="s">
         <v>130</v>
       </c>
@@ -5788,8 +5836,8 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="184"/>
-      <c r="B28" s="184"/>
+      <c r="A28" s="162"/>
+      <c r="B28" s="162"/>
       <c r="C28" s="28" t="s">
         <v>129</v>
       </c>
@@ -6018,10 +6066,10 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="187" t="s">
+      <c r="A3" s="165" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="184" t="s">
+      <c r="B3" s="162" t="s">
         <v>61</v>
       </c>
       <c r="C3" s="16" t="s">
@@ -6032,8 +6080,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="38.25" x14ac:dyDescent="0.3">
-      <c r="A4" s="187"/>
-      <c r="B4" s="184"/>
+      <c r="A4" s="165"/>
+      <c r="B4" s="162"/>
       <c r="C4" s="16" t="s">
         <v>64</v>
       </c>
@@ -6042,8 +6090,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
-      <c r="A5" s="187"/>
-      <c r="B5" s="184"/>
+      <c r="A5" s="165"/>
+      <c r="B5" s="162"/>
       <c r="C5" s="16" t="s">
         <v>65</v>
       </c>
@@ -6052,8 +6100,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="187"/>
-      <c r="B6" s="184"/>
+      <c r="A6" s="165"/>
+      <c r="B6" s="162"/>
       <c r="C6" s="16" t="s">
         <v>66</v>
       </c>
@@ -6062,8 +6110,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="187"/>
-      <c r="B7" s="184"/>
+      <c r="A7" s="165"/>
+      <c r="B7" s="162"/>
       <c r="C7" s="16" t="s">
         <v>67</v>
       </c>
@@ -6072,8 +6120,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="187"/>
-      <c r="B8" s="184"/>
+      <c r="A8" s="165"/>
+      <c r="B8" s="162"/>
       <c r="C8" s="16" t="s">
         <v>68</v>
       </c>
@@ -6082,8 +6130,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="187"/>
-      <c r="B9" s="184"/>
+      <c r="A9" s="165"/>
+      <c r="B9" s="162"/>
       <c r="C9" s="16" t="s">
         <v>69</v>
       </c>
@@ -6092,8 +6140,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="187"/>
-      <c r="B10" s="184"/>
+      <c r="A10" s="165"/>
+      <c r="B10" s="162"/>
       <c r="C10" s="16" t="s">
         <v>70</v>
       </c>
@@ -6102,8 +6150,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="187"/>
-      <c r="B11" s="184"/>
+      <c r="A11" s="165"/>
+      <c r="B11" s="162"/>
       <c r="C11" s="16" t="s">
         <v>71</v>
       </c>
@@ -6112,8 +6160,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="187"/>
-      <c r="B12" s="184"/>
+      <c r="A12" s="165"/>
+      <c r="B12" s="162"/>
       <c r="C12" s="16" t="s">
         <v>72</v>
       </c>
@@ -6122,8 +6170,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="188"/>
-      <c r="B13" s="189"/>
+      <c r="A13" s="166"/>
+      <c r="B13" s="167"/>
       <c r="C13" s="24" t="s">
         <v>73</v>
       </c>
@@ -6132,10 +6180,10 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="186" t="s">
+      <c r="A14" s="164" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="185" t="s">
+      <c r="B14" s="163" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="22" t="s">
@@ -6144,8 +6192,8 @@
       <c r="D14" s="23"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="187"/>
-      <c r="B15" s="184"/>
+      <c r="A15" s="165"/>
+      <c r="B15" s="162"/>
       <c r="C15" s="16" t="s">
         <v>75</v>
       </c>
@@ -6154,8 +6202,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
-      <c r="A16" s="187"/>
-      <c r="B16" s="184"/>
+      <c r="A16" s="165"/>
+      <c r="B16" s="162"/>
       <c r="C16" s="16" t="s">
         <v>71</v>
       </c>
@@ -6164,8 +6212,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="187"/>
-      <c r="B17" s="184"/>
+      <c r="A17" s="165"/>
+      <c r="B17" s="162"/>
       <c r="C17" s="16" t="s">
         <v>76</v>
       </c>
@@ -6174,8 +6222,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="187"/>
-      <c r="B18" s="184"/>
+      <c r="A18" s="165"/>
+      <c r="B18" s="162"/>
       <c r="C18" s="16" t="s">
         <v>64</v>
       </c>
@@ -6184,8 +6232,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="187"/>
-      <c r="B19" s="184"/>
+      <c r="A19" s="165"/>
+      <c r="B19" s="162"/>
       <c r="C19" s="16" t="s">
         <v>77</v>
       </c>
@@ -6194,8 +6242,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
-      <c r="A20" s="187"/>
-      <c r="B20" s="184"/>
+      <c r="A20" s="165"/>
+      <c r="B20" s="162"/>
       <c r="C20" s="16" t="s">
         <v>67</v>
       </c>
@@ -6204,8 +6252,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="187"/>
-      <c r="B21" s="184"/>
+      <c r="A21" s="165"/>
+      <c r="B21" s="162"/>
       <c r="C21" s="16" t="s">
         <v>78</v>
       </c>
@@ -6214,8 +6262,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="187"/>
-      <c r="B22" s="184"/>
+      <c r="A22" s="165"/>
+      <c r="B22" s="162"/>
       <c r="C22" s="16" t="s">
         <v>79</v>
       </c>
@@ -6224,8 +6272,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="187"/>
-      <c r="B23" s="184"/>
+      <c r="A23" s="165"/>
+      <c r="B23" s="162"/>
       <c r="C23" s="16" t="s">
         <v>80</v>
       </c>
@@ -6234,8 +6282,8 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="187"/>
-      <c r="B24" s="184"/>
+      <c r="A24" s="165"/>
+      <c r="B24" s="162"/>
       <c r="C24" s="16" t="s">
         <v>81</v>
       </c>
@@ -6244,16 +6292,16 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="187"/>
-      <c r="B25" s="184"/>
+      <c r="A25" s="165"/>
+      <c r="B25" s="162"/>
       <c r="C25" s="16" t="s">
         <v>82</v>
       </c>
       <c r="D25" s="19"/>
     </row>
     <row r="26" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="187"/>
-      <c r="B26" s="184"/>
+      <c r="A26" s="165"/>
+      <c r="B26" s="162"/>
       <c r="C26" s="16" t="s">
         <v>34</v>
       </c>
@@ -6262,8 +6310,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
-      <c r="A27" s="187"/>
-      <c r="B27" s="184"/>
+      <c r="A27" s="165"/>
+      <c r="B27" s="162"/>
       <c r="C27" s="16" t="s">
         <v>83</v>
       </c>
@@ -6272,8 +6320,8 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="187"/>
-      <c r="B28" s="184"/>
+      <c r="A28" s="165"/>
+      <c r="B28" s="162"/>
       <c r="C28" s="16" t="s">
         <v>84</v>
       </c>
@@ -6282,8 +6330,8 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="187"/>
-      <c r="B29" s="184"/>
+      <c r="A29" s="165"/>
+      <c r="B29" s="162"/>
       <c r="C29" s="16" t="s">
         <v>85</v>
       </c>

</xml_diff>